<commit_message>
refactor Pendulum.py to enhance linear regression calculations and include uncertainty analysis
</commit_message>
<xml_diff>
--- a/data/Dane.xlsx
+++ b/data/Dane.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuba-\Desktop\simple_graph_tool_xdf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25C0C9E-3608-479D-8D6D-28760794BAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDFDA20-4745-4E60-B323-1FFA948DF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="4470" windowWidth="21600" windowHeight="11295" xr2:uid="{38249783-EF5F-485F-9AB0-331F4EBD13C0}"/>
+    <workbookView xWindow="2895" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{38249783-EF5F-485F-9AB0-331F4EBD13C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>t1 [s]</t>
-  </si>
-  <si>
-    <t>t2 [s]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>T</t>
   </si>
@@ -51,24 +45,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D </t>
-  </si>
-  <si>
-    <t>+/- 0,01 m</t>
-  </si>
-  <si>
-    <t>+/- 0,6</t>
-  </si>
-  <si>
-    <t>m [kg] +/-0,03</t>
   </si>
   <si>
     <t>D</t>
@@ -467,7 +443,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G1" sqref="G1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,41 +454,29 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -533,24 +497,12 @@
       <c r="F2" s="3">
         <v>0.20887475599999999</v>
       </c>
-      <c r="G2" s="2">
-        <v>12.75114101</v>
-      </c>
-      <c r="H2" s="1">
-        <v>-7.1303284999999994E-2</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0.78300000000000003</v>
-      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">

</xml_diff>

<commit_message>
fix uncertainty calculation and update plot labels for clarity in Pendulum.py
</commit_message>
<xml_diff>
--- a/data/Dane.xlsx
+++ b/data/Dane.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuba-\Desktop\simple_graph_tool_xdf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDFDA20-4745-4E60-B323-1FFA948DF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAD3218-98D4-4E52-AFDF-C2A9D7C67F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{38249783-EF5F-485F-9AB0-331F4EBD13C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{38249783-EF5F-485F-9AB0-331F4EBD13C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,18 +97,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -124,9 +121,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -164,7 +161,7 @@
         <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
@@ -270,7 +267,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -443,7 +440,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:M1"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,240 +468,227 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="2">
+        <f xml:space="preserve"> 0.45 -0.1</f>
+        <v>0.35</v>
+      </c>
+      <c r="B2" s="2">
         <v>28.91</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>28.9</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>1.4452499999999999</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0.01</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0.20887475599999999</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="A3" s="2">
+        <f xml:space="preserve"> 0.45 -0.13</f>
+        <v>0.32</v>
+      </c>
+      <c r="B3" s="2">
         <v>28.58</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>29.11</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1.44225</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1.6899999999999998E-2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.27041105799999998</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" s="2">
+        <f xml:space="preserve"> 0.45 -0.16</f>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="B4" s="2">
         <v>28.79</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>28.8</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>1.4397500000000001</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.33166080999999997</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" s="2">
+        <f xml:space="preserve"> 0.45 -0.19</f>
+        <v>0.26</v>
+      </c>
+      <c r="B5" s="2">
         <v>29.21</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>28.93</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1.4535</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>3.61E-2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0.40140582800000002</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="A6" s="2">
+        <f xml:space="preserve"> 0.45 -0.22</f>
+        <v>0.23</v>
+      </c>
+      <c r="B6" s="2">
         <v>29.26</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>29.39</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>1.4662500000000001</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>4.8399999999999999E-2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>0.472975594</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="B7" s="3">
+      <c r="A7" s="2">
+        <f xml:space="preserve"> 0.45 -0.25</f>
+        <v>0.2</v>
+      </c>
+      <c r="B7" s="2">
         <v>30.71</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>30.44</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>1.5287500000000001</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>0.58426914100000005</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="B8" s="3">
+      <c r="A8" s="2">
+        <f xml:space="preserve"> 0.45 -0.28</f>
+        <v>0.16999999999999998</v>
+      </c>
+      <c r="B8" s="2">
         <v>31.24</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>31.47</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>1.56775</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>7.8399999999999997E-2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>0.68819521800000005</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>0.31</v>
-      </c>
-      <c r="B9" s="3">
+      <c r="A9" s="2">
+        <f xml:space="preserve"> 0.45 -0.31</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="B9" s="2">
         <v>34.24</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>34.04</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1.7070000000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>9.6100000000000005E-2</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>0.90329318999999997</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>0.34</v>
-      </c>
-      <c r="B10" s="3">
+      <c r="A10" s="2">
+        <f xml:space="preserve"> 0.45 -0.34</f>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="B10" s="2">
         <v>38.17</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>38.19</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>1.909</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>0.11559999999999999</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>1.2390555400000001</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>0.37</v>
-      </c>
-      <c r="B11" s="3">
+      <c r="A11" s="2">
+        <f xml:space="preserve"> 0.45 -0.37</f>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="B11" s="2">
         <v>48.26</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>48.38</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>2.4159999999999999</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>0.13689999999999999</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>2.1597107200000001</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>

</xml_diff>